<commit_message>
Preparing ExcelDataImporter class to export the records into an excel. Also Added apache-poi jars.
</commit_message>
<xml_diff>
--- a/com.rise.daemon/database/Person.xlsx
+++ b/com.rise.daemon/database/Person.xlsx
@@ -12,12 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="64">
-  <si>
-    <t>dateOfBirth</t>
-  </si>
-  <si>
-    <t>aadhaarNumber</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="60">
+  <si>
+    <t/>
   </si>
   <si>
     <t>EDU-name</t>
@@ -104,18 +101,12 @@
     <t>AWARD-description</t>
   </si>
   <si>
-    <t>9874563210</t>
-  </si>
-  <si>
     <t>Bcom</t>
   </si>
   <si>
     <t>JNTU</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Bsc</t>
   </si>
   <si>
@@ -162,9 +153,6 @@
   </si>
   <si>
     <t>For Best Services...</t>
-  </si>
-  <si>
-    <t>123456780178</t>
   </si>
   <si>
     <t>Bsc Computers</t>
@@ -244,6 +232,22 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -343,441 +347,424 @@
       <c r="AC1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="n">
+        <v>2007.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>68.0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="n">
         <v>32579.0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2007.0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>68.0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="I2" t="s">
-        <v>38</v>
       </c>
       <c r="J2" t="n">
         <v>32579.0</v>
       </c>
-      <c r="K2" t="n">
-        <v>32579.0</v>
+      <c r="K2" t="s">
+        <v>36</v>
       </c>
       <c r="L2" t="s">
+        <v>36</v>
+      </c>
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA2" t="s">
         <v>39</v>
       </c>
-      <c r="M2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" t="s">
-        <v>33</v>
-      </c>
-      <c r="V2" t="s">
-        <v>33</v>
-      </c>
-      <c r="W2" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC2" t="n">
+      <c r="AB2" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD2" t="s">
-        <v>43</v>
+      <c r="AC2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2007.0</v>
       </c>
       <c r="E3" t="n">
-        <v>2007.0</v>
+        <v>13.0</v>
       </c>
       <c r="F3" t="n">
-        <v>13.0</v>
+        <v>68.0</v>
       </c>
       <c r="G3" t="n">
-        <v>68.0</v>
-      </c>
-      <c r="H3" t="n">
         <v>80.0</v>
       </c>
-      <c r="I3" t="s">
-        <v>40</v>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="n">
+        <v>32579.0</v>
       </c>
       <c r="J3" t="n">
         <v>32579.0</v>
       </c>
-      <c r="K3" t="n">
-        <v>32579.0</v>
+      <c r="K3" t="s">
+        <v>36</v>
       </c>
       <c r="L3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>41</v>
       </c>
       <c r="AA3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC3" t="n">
+        <v>42</v>
+      </c>
+      <c r="AB3" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD3" t="s">
-        <v>46</v>
+      <c r="AC3" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
+        <v>32</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2009.0</v>
       </c>
       <c r="E4" t="n">
-        <v>2009.0</v>
+        <v>6.0</v>
       </c>
       <c r="F4" t="n">
-        <v>6.0</v>
+        <v>75.0</v>
       </c>
       <c r="G4" t="n">
-        <v>75.0</v>
-      </c>
-      <c r="H4" t="n">
         <v>7.5</v>
       </c>
+      <c r="Z4" t="s">
+        <v>44</v>
+      </c>
       <c r="AA4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC4" t="n">
+        <v>45</v>
+      </c>
+      <c r="AB4" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD4" t="s">
-        <v>49</v>
+      <c r="AC4" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
         <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2010.0</v>
       </c>
       <c r="E5" t="n">
-        <v>2010.0</v>
+        <v>6.0</v>
       </c>
       <c r="F5" t="n">
-        <v>6.0</v>
+        <v>85.0</v>
       </c>
       <c r="G5" t="n">
-        <v>85.0</v>
-      </c>
-      <c r="H5" t="n">
         <v>8.5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2006.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>77.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7.699999809265137</v>
+      </c>
+      <c r="H6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I6" t="n">
         <v>32579.0</v>
-      </c>
-      <c r="B6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="n">
-        <v>2006.0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>77.0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>7.699999809265137</v>
-      </c>
-      <c r="I6" t="s">
-        <v>58</v>
       </c>
       <c r="J6" t="n">
         <v>32579.0</v>
       </c>
-      <c r="K6" t="n">
-        <v>32579.0</v>
+      <c r="K6" t="s">
+        <v>36</v>
       </c>
       <c r="L6" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="M6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S6" t="s">
+        <v>0</v>
+      </c>
+      <c r="T6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" t="s">
+        <v>0</v>
+      </c>
+      <c r="W6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>38051.0</v>
+      </c>
+      <c r="AC6" t="s">
         <v>59</v>
-      </c>
-      <c r="N6" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>33</v>
-      </c>
-      <c r="R6" t="s">
-        <v>33</v>
-      </c>
-      <c r="S6" t="s">
-        <v>33</v>
-      </c>
-      <c r="T6" t="s">
-        <v>33</v>
-      </c>
-      <c r="U6" t="s">
-        <v>33</v>
-      </c>
-      <c r="V6" t="s">
-        <v>33</v>
-      </c>
-      <c r="W6" t="s">
-        <v>33</v>
-      </c>
-      <c r="X6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z6" t="s">
-        <v>33</v>
-      </c>
-      <c r="AA6" t="s">
-        <v>61</v>
-      </c>
-      <c r="AB6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>38051.0</v>
-      </c>
-      <c r="AD6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2010.0</v>
       </c>
       <c r="E7" t="n">
-        <v>2010.0</v>
+        <v>5.0</v>
       </c>
       <c r="F7" t="n">
-        <v>5.0</v>
+        <v>80.0</v>
       </c>
       <c r="G7" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="H7" t="n">
         <v>8.0</v>
       </c>
-      <c r="I7" t="s">
-        <v>60</v>
+      <c r="H7" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" t="n">
+        <v>32579.0</v>
       </c>
       <c r="J7" t="n">
         <v>32579.0</v>
       </c>
-      <c r="K7" t="n">
-        <v>32579.0</v>
+      <c r="K7" t="s">
+        <v>55</v>
       </c>
       <c r="L7" t="s">
-        <v>59</v>
-      </c>
-      <c r="M7" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>44</v>
       </c>
       <c r="AA7" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC7" t="n">
+        <v>45</v>
+      </c>
+      <c r="AB7" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD7" t="s">
-        <v>49</v>
+      <c r="AC7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" t="s">
-        <v>55</v>
+        <v>51</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2004.0</v>
       </c>
       <c r="E8" t="n">
-        <v>2004.0</v>
+        <v>4.0</v>
       </c>
       <c r="F8" t="n">
-        <v>4.0</v>
+        <v>80.0</v>
       </c>
       <c r="G8" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="H8" t="n">
         <v>8.050000190734863</v>
       </c>
+      <c r="Z8" t="s">
+        <v>38</v>
+      </c>
       <c r="AA8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC8" t="n">
+        <v>39</v>
+      </c>
+      <c r="AB8" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD8" t="s">
-        <v>43</v>
+      <c r="AC8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2002.0</v>
       </c>
       <c r="E9" t="n">
-        <v>2002.0</v>
+        <v>3.0</v>
       </c>
       <c r="F9" t="n">
-        <v>3.0</v>
+        <v>78.0</v>
       </c>
       <c r="G9" t="n">
-        <v>78.0</v>
-      </c>
-      <c r="H9" t="n">
         <v>7.800000190734863</v>
       </c>
+      <c r="Z9" t="s">
+        <v>41</v>
+      </c>
       <c r="AA9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC9" t="n">
+        <v>42</v>
+      </c>
+      <c r="AB9" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD9" t="s">
-        <v>46</v>
+      <c r="AC9" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:Z100">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(),5)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:Z100">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(),5)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added TAB annotation and also developing a dynamic jsp...
</commit_message>
<xml_diff>
--- a/com.rise.daemon/database/Person.xlsx
+++ b/com.rise.daemon/database/Person.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="78">
   <si>
     <t>dateOfBirth</t>
   </si>
@@ -20,6 +20,21 @@
     <t>aadhaarNumber</t>
   </si>
   <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>firstName</t>
+  </si>
+  <si>
+    <t>middleName</t>
+  </si>
+  <si>
+    <t>lastName</t>
+  </si>
+  <si>
+    <t>suffix</t>
+  </si>
+  <si>
     <t>EDU-name</t>
   </si>
   <si>
@@ -107,13 +122,13 @@
     <t>9874563210</t>
   </si>
   <si>
+    <t/>
+  </si>
+  <si>
     <t>Bcom</t>
   </si>
   <si>
     <t>JNTU</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>Bsc</t>
@@ -229,6 +244,9 @@
   </si>
   <si>
     <t>123456699123</t>
+  </si>
+  <si>
+    <t>123456699123456</t>
   </si>
 </sst>
 </file>
@@ -268,7 +286,14 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="42"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -442,213 +467,288 @@
       <c r="AD1" t="s">
         <v>29</v>
       </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
         <v>32579.0</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2007.0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="G2" t="n">
-        <v>68.0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>8.0</v>
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" t="s">
+        <v>37</v>
       </c>
       <c r="I2" t="s">
         <v>38</v>
       </c>
       <c r="J2" t="n">
+        <v>2007.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>68.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" t="n">
         <v>32579.0</v>
       </c>
-      <c r="K2" t="n">
+      <c r="P2" t="n">
         <v>32579.0</v>
       </c>
-      <c r="L2" t="s">
-        <v>39</v>
-      </c>
-      <c r="M2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" t="s">
-        <v>33</v>
-      </c>
       <c r="Q2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="R2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="S2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="W2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="X2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Y2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Z2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AA2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="AB2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC2" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH2" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD2" t="s">
-        <v>43</v>
+      <c r="AI2" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="n">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" t="n">
         <v>2007.0</v>
       </c>
-      <c r="F3" t="n">
+      <c r="K3" t="n">
         <v>13.0</v>
       </c>
-      <c r="G3" t="n">
+      <c r="L3" t="n">
         <v>68.0</v>
       </c>
-      <c r="H3" t="n">
+      <c r="M3" t="n">
         <v>80.0</v>
       </c>
-      <c r="I3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J3" t="n">
+      <c r="N3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" t="n">
         <v>32579.0</v>
       </c>
-      <c r="K3" t="n">
+      <c r="P3" t="n">
         <v>32579.0</v>
       </c>
-      <c r="L3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M3" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA3" t="s">
+      <c r="Q3" t="s">
         <v>44</v>
       </c>
-      <c r="AB3" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC3" t="n">
+      <c r="R3" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH3" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD3" t="s">
-        <v>46</v>
+      <c r="AI3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" t="n">
+        <v>36</v>
+      </c>
+      <c r="E4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="n">
         <v>2009.0</v>
       </c>
-      <c r="F4" t="n">
+      <c r="K4" t="n">
         <v>6.0</v>
       </c>
-      <c r="G4" t="n">
+      <c r="L4" t="n">
         <v>75.0</v>
       </c>
-      <c r="H4" t="n">
+      <c r="M4" t="n">
         <v>7.5</v>
       </c>
-      <c r="AA4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC4" t="n">
+      <c r="AF4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH4" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD4" t="s">
-        <v>49</v>
+      <c r="AI4" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
         <v>36</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="n">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="n">
         <v>2010.0</v>
       </c>
-      <c r="F5" t="n">
+      <c r="K5" t="n">
         <v>6.0</v>
       </c>
-      <c r="G5" t="n">
+      <c r="L5" t="n">
         <v>85.0</v>
       </c>
-      <c r="H5" t="n">
+      <c r="M5" t="n">
         <v>8.5</v>
       </c>
     </row>
@@ -657,220 +757,280 @@
         <v>32579.0</v>
       </c>
       <c r="B6" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="n">
+        <v>36</v>
+      </c>
+      <c r="E6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" t="n">
         <v>2006.0</v>
       </c>
-      <c r="F6" t="n">
+      <c r="K6" t="n">
         <v>7.0</v>
       </c>
-      <c r="G6" t="n">
+      <c r="L6" t="n">
         <v>77.0</v>
       </c>
-      <c r="H6" t="n">
+      <c r="M6" t="n">
         <v>7.699999809265137</v>
       </c>
-      <c r="I6" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" t="n">
+      <c r="N6" t="s">
+        <v>63</v>
+      </c>
+      <c r="O6" t="n">
         <v>32579.0</v>
       </c>
-      <c r="K6" t="n">
+      <c r="P6" t="n">
         <v>32579.0</v>
       </c>
-      <c r="L6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M6" t="s">
-        <v>59</v>
-      </c>
-      <c r="N6" t="s">
-        <v>33</v>
-      </c>
-      <c r="O6" t="s">
-        <v>33</v>
-      </c>
-      <c r="P6" t="s">
-        <v>33</v>
-      </c>
       <c r="Q6" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="R6" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="S6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="W6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="X6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Y6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Z6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AA6" t="s">
-        <v>61</v>
+        <v>36</v>
       </c>
       <c r="AB6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC6" t="n">
+        <v>36</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH6" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD6" t="s">
-        <v>63</v>
+      <c r="AI6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="n">
+        <v>2010.0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="M7" t="n">
+        <v>8.0</v>
+      </c>
+      <c r="N7" t="s">
+        <v>65</v>
+      </c>
+      <c r="O7" t="n">
+        <v>32579.0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>32579.0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>64</v>
+      </c>
+      <c r="R7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AG7" t="s">
         <v>53</v>
       </c>
-      <c r="D7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="n">
-        <v>2010.0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="G7" t="n">
-        <v>80.0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>8.0</v>
-      </c>
-      <c r="I7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J7" t="n">
-        <v>32579.0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>32579.0</v>
-      </c>
-      <c r="L7" t="s">
-        <v>59</v>
-      </c>
-      <c r="M7" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA7" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB7" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC7" t="n">
+      <c r="AH7" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD7" t="s">
-        <v>49</v>
+      <c r="AI7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" t="n">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" t="n">
         <v>2004.0</v>
       </c>
-      <c r="F8" t="n">
+      <c r="K8" t="n">
         <v>4.0</v>
       </c>
-      <c r="G8" t="n">
+      <c r="L8" t="n">
         <v>80.0</v>
       </c>
-      <c r="H8" t="n">
+      <c r="M8" t="n">
         <v>8.050000190734863</v>
       </c>
-      <c r="AA8" t="s">
-        <v>41</v>
-      </c>
-      <c r="AB8" t="s">
-        <v>42</v>
-      </c>
-      <c r="AC8" t="n">
+      <c r="AF8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH8" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD8" t="s">
-        <v>43</v>
+      <c r="AI8" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" t="n">
+        <v>36</v>
+      </c>
+      <c r="E9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" t="s">
+        <v>61</v>
+      </c>
+      <c r="I9" t="s">
+        <v>62</v>
+      </c>
+      <c r="J9" t="n">
         <v>2002.0</v>
       </c>
-      <c r="F9" t="n">
+      <c r="K9" t="n">
         <v>3.0</v>
       </c>
-      <c r="G9" t="n">
+      <c r="L9" t="n">
         <v>78.0</v>
       </c>
-      <c r="H9" t="n">
+      <c r="M9" t="n">
         <v>7.800000190734863</v>
       </c>
-      <c r="AA9" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB9" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC9" t="n">
+      <c r="AF9" t="s">
+        <v>49</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>50</v>
+      </c>
+      <c r="AH9" t="n">
         <v>38051.0</v>
       </c>
-      <c r="AD9" t="s">
-        <v>46</v>
+      <c r="AI9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10">
@@ -878,91 +1038,106 @@
         <v>32579.0</v>
       </c>
       <c r="B10" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="W10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="X10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Y10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Z10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AA10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AB10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AC10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AD10" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11">
@@ -970,91 +1145,106 @@
         <v>32579.0</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="W11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="X11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Y11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Z11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AA11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AB11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AC11" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AD11" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12">
@@ -1062,91 +1252,106 @@
         <v>32579.0</v>
       </c>
       <c r="B12" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="W12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="X12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Y12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Z12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AA12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AB12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AC12" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AD12" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13">
@@ -1154,91 +1359,106 @@
         <v>24543.0</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="W13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="X13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Y13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Z13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AA13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AB13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AC13" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AD13" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14">
@@ -1246,91 +1466,106 @@
         <v>24543.0</v>
       </c>
       <c r="B14" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="W14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="X14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Y14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Z14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AA14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AB14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AC14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AD14" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15">
@@ -1338,91 +1573,106 @@
         <v>24543.0</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="W15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="X15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Y15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Z15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AA15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AB15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AC15" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AD15" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="16">
@@ -1430,91 +1680,106 @@
         <v>24543.0</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="W16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="X16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Y16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Z16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AA16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AB16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AC16" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AD16" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17">
@@ -1522,91 +1787,213 @@
         <v>32579.0</v>
       </c>
       <c r="B17" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="I17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="K17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="L17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="M17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="N17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="O17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="P17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Q17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="R17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="S17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="T17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="U17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="V17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="W17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="X17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Y17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="Z17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AA17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AB17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AC17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="AD17" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>32579.0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G18" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" t="s">
+        <v>36</v>
+      </c>
+      <c r="J18" t="s">
+        <v>36</v>
+      </c>
+      <c r="K18" t="s">
+        <v>36</v>
+      </c>
+      <c r="L18" t="s">
+        <v>36</v>
+      </c>
+      <c r="M18" t="s">
+        <v>36</v>
+      </c>
+      <c r="N18" t="s">
+        <v>36</v>
+      </c>
+      <c r="O18" t="s">
+        <v>36</v>
+      </c>
+      <c r="P18" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>36</v>
+      </c>
+      <c r="R18" t="s">
+        <v>36</v>
+      </c>
+      <c r="S18" t="s">
+        <v>36</v>
+      </c>
+      <c r="T18" t="s">
+        <v>36</v>
+      </c>
+      <c r="U18" t="s">
+        <v>36</v>
+      </c>
+      <c r="V18" t="s">
+        <v>36</v>
+      </c>
+      <c r="W18" t="s">
+        <v>36</v>
+      </c>
+      <c r="X18" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1660,6 +2047,11 @@
       <formula>MOD(ROW(),5)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A1:Z100">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>MOD(ROW(),5)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>